<commit_message>
Converting more to graph
</commit_message>
<xml_diff>
--- a/Data/xlsx/basal_ganglia_cells.xlsx
+++ b/Data/xlsx/basal_ganglia_cells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\uio\master\jup_bg\Data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51843757-A11E-420D-996C-EEE78E884485}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17F6BFD-2616-4A97-AEED-820F36A6DD2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-1974" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="5" xr2:uid="{1FF931E2-FF21-450C-9096-8D433BB6F073}"/>
   </bookViews>
@@ -17,8 +17,10 @@
     <sheet name="Cell_phenotypes" sheetId="3" r:id="rId2"/>
     <sheet name="Cell_type_classifications" sheetId="4" r:id="rId3"/>
     <sheet name="Cell_types" sheetId="5" r:id="rId4"/>
-    <sheet name="cell_phenotype_type_categories" sheetId="2" r:id="rId5"/>
-    <sheet name="celltypes_phenotypes" sheetId="6" r:id="rId6"/>
+    <sheet name="Cellular_regions" sheetId="7" r:id="rId5"/>
+    <sheet name="Objects_of_interest" sheetId="8" r:id="rId6"/>
+    <sheet name="cell_phenotype_type_categories" sheetId="2" r:id="rId7"/>
+    <sheet name="celltypes_phenotypes" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3527" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="947">
   <si>
     <t>ID</t>
   </si>
@@ -2757,6 +2759,126 @@
   </si>
   <si>
     <t>CellID</t>
+  </si>
+  <si>
+    <t>Cellular_region</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>NLX:154731</t>
+  </si>
+  <si>
+    <t>Distal dendrite</t>
+  </si>
+  <si>
+    <t>NLX:154733</t>
+  </si>
+  <si>
+    <t>Proximal dendrite</t>
+  </si>
+  <si>
+    <t>NLX:154734</t>
+  </si>
+  <si>
+    <t>Dendrite</t>
+  </si>
+  <si>
+    <t>SAO:1211023249</t>
+  </si>
+  <si>
+    <t>Dendritic spine</t>
+  </si>
+  <si>
+    <t>GO:0043197</t>
+  </si>
+  <si>
+    <t>Dendritic shaft</t>
+  </si>
+  <si>
+    <t>SAO:2034472720</t>
+  </si>
+  <si>
+    <t>Vesicle containing profile</t>
+  </si>
+  <si>
+    <t>Dendritic region, unspecified</t>
+  </si>
+  <si>
+    <t>Somatodendritic domain</t>
+  </si>
+  <si>
+    <t>Object_of_interest</t>
+  </si>
+  <si>
+    <t>Neurons</t>
+  </si>
+  <si>
+    <t>Cells</t>
+  </si>
+  <si>
+    <t>ILX:0101839</t>
+  </si>
+  <si>
+    <t>Axonal terminals</t>
+  </si>
+  <si>
+    <t>ILX:0101049</t>
+  </si>
+  <si>
+    <t>Synapses</t>
+  </si>
+  <si>
+    <t>GO:0045202</t>
+  </si>
+  <si>
+    <t>Synapses, symmetrical</t>
+  </si>
+  <si>
+    <t>ILX:0111392</t>
+  </si>
+  <si>
+    <t>Synapses, asymmetrical</t>
+  </si>
+  <si>
+    <t>ILX:0100953</t>
+  </si>
+  <si>
+    <t>Dendritic spines</t>
+  </si>
+  <si>
+    <t>Dendritic spines, mushroom</t>
+  </si>
+  <si>
+    <t>ILX:0107249</t>
+  </si>
+  <si>
+    <t>Dendritic spines, stubby</t>
+  </si>
+  <si>
+    <t>ILX:0111129</t>
+  </si>
+  <si>
+    <t>Dendritic spines, thin</t>
+  </si>
+  <si>
+    <t>ILX:0111691</t>
+  </si>
+  <si>
+    <t>Dendritic spines, large</t>
+  </si>
+  <si>
+    <t>Dendritic spines, giant</t>
+  </si>
+  <si>
+    <t>Glia cell</t>
+  </si>
+  <si>
+    <t>Axonal varicosities</t>
   </si>
 </sst>
 </file>
@@ -12778,6 +12900,359 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53F2515-A32A-40EC-91F1-F335698B6CFD}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>909</v>
+      </c>
+      <c r="C2" t="s">
+        <v>910</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>911</v>
+      </c>
+      <c r="C3" t="s">
+        <v>912</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>913</v>
+      </c>
+      <c r="C4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>915</v>
+      </c>
+      <c r="C5" t="s">
+        <v>916</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>917</v>
+      </c>
+      <c r="C6" t="s">
+        <v>918</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>919</v>
+      </c>
+      <c r="C7" t="s">
+        <v>920</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>921</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>922</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>923</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>820</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F4C332-94C0-4331-9628-741E083E8E8D}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C2" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>926</v>
+      </c>
+      <c r="C3" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>928</v>
+      </c>
+      <c r="C4" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>930</v>
+      </c>
+      <c r="C5" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>932</v>
+      </c>
+      <c r="C6" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>934</v>
+      </c>
+      <c r="C7" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>936</v>
+      </c>
+      <c r="C8" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>937</v>
+      </c>
+      <c r="C9" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>939</v>
+      </c>
+      <c r="C10" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>941</v>
+      </c>
+      <c r="C11" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>943</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>944</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>945</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>946</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F959E716-4AC9-48E5-A4FE-D4B91DF01C49}">
   <dimension ref="A1:F591"/>
   <sheetViews>
@@ -24612,11 +25087,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB7EC8D-C3E0-452A-9449-EA7E80D4441B}">
   <dimension ref="A1:D578"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
graph and removed some celltypes
</commit_message>
<xml_diff>
--- a/Data/xlsx/basal_ganglia_cells.xlsx
+++ b/Data/xlsx/basal_ganglia_cells.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\uio\master\jup_bg\Data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B883F375-3FFD-4603-A0B2-6B066AB51A75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6715882-E6A9-4AFE-A1EB-35D4F2FE2EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{1FF931E2-FF21-450C-9096-8D433BB6F073}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3518" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="960">
   <si>
     <t>ID</t>
   </si>
@@ -2460,9 +2460,6 @@
     <t>Dopamine receptor 3 expressing / enkephalin negative</t>
   </si>
   <si>
-    <t>Substance P / PPA co-expressing</t>
-  </si>
-  <si>
     <t>Dopamine receptor 2  / enkephalin co-expressing</t>
   </si>
   <si>
@@ -2653,9 +2650,6 @@
   </si>
   <si>
     <t>Outer globus pallidus neuron</t>
-  </si>
-  <si>
-    <t>PSA-NCAM expressing</t>
   </si>
   <si>
     <t>Somatostatin / calretinin co-expressing</t>
@@ -3369,13 +3363,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D1" t="s">
         <v>792</v>
@@ -6752,7 +6746,7 @@
         <v>29</v>
       </c>
       <c r="D242" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -6766,7 +6760,7 @@
         <v>29</v>
       </c>
       <c r="D243" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -6780,7 +6774,7 @@
         <v>30</v>
       </c>
       <c r="D244" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -6794,7 +6788,7 @@
         <v>30</v>
       </c>
       <c r="D245" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -6808,7 +6802,7 @@
         <v>31</v>
       </c>
       <c r="D246" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -6822,7 +6816,7 @@
         <v>31</v>
       </c>
       <c r="D247" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -6836,7 +6830,7 @@
         <v>33</v>
       </c>
       <c r="D248" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -6850,7 +6844,7 @@
         <v>33</v>
       </c>
       <c r="D249" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -6864,7 +6858,7 @@
         <v>33</v>
       </c>
       <c r="D250" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -6878,7 +6872,7 @@
         <v>33</v>
       </c>
       <c r="D251" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -6892,7 +6886,7 @@
         <v>33</v>
       </c>
       <c r="D252" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -6906,7 +6900,7 @@
         <v>33</v>
       </c>
       <c r="D253" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -6920,7 +6914,7 @@
         <v>33</v>
       </c>
       <c r="D254" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -6934,7 +6928,7 @@
         <v>33</v>
       </c>
       <c r="D255" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -6948,7 +6942,7 @@
         <v>33</v>
       </c>
       <c r="D256" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,7 +6956,7 @@
         <v>33</v>
       </c>
       <c r="D257" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -6976,7 +6970,7 @@
         <v>33</v>
       </c>
       <c r="D258" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6990,7 +6984,7 @@
         <v>33</v>
       </c>
       <c r="D259" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -7004,7 +6998,7 @@
         <v>33</v>
       </c>
       <c r="D260" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -7018,7 +7012,7 @@
         <v>33</v>
       </c>
       <c r="D261" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -7032,7 +7026,7 @@
         <v>33</v>
       </c>
       <c r="D262" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -7046,7 +7040,7 @@
         <v>33</v>
       </c>
       <c r="D263" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -7060,7 +7054,7 @@
         <v>33</v>
       </c>
       <c r="D264" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -7074,7 +7068,7 @@
         <v>33</v>
       </c>
       <c r="D265" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -7088,7 +7082,7 @@
         <v>33</v>
       </c>
       <c r="D266" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -7102,7 +7096,7 @@
         <v>33</v>
       </c>
       <c r="D267" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -7116,7 +7110,7 @@
         <v>33</v>
       </c>
       <c r="D268" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -7130,7 +7124,7 @@
         <v>33</v>
       </c>
       <c r="D269" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -7144,7 +7138,7 @@
         <v>33</v>
       </c>
       <c r="D270" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -7158,7 +7152,7 @@
         <v>33</v>
       </c>
       <c r="D271" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -7172,7 +7166,7 @@
         <v>33</v>
       </c>
       <c r="D272" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -7186,7 +7180,7 @@
         <v>33</v>
       </c>
       <c r="D273" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -7200,7 +7194,7 @@
         <v>34</v>
       </c>
       <c r="D274" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -7214,7 +7208,7 @@
         <v>36</v>
       </c>
       <c r="D275" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -7228,7 +7222,7 @@
         <v>36</v>
       </c>
       <c r="D276" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -7242,7 +7236,7 @@
         <v>36</v>
       </c>
       <c r="D277" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -7256,7 +7250,7 @@
         <v>36</v>
       </c>
       <c r="D278" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -7270,7 +7264,7 @@
         <v>36</v>
       </c>
       <c r="D279" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -7284,7 +7278,7 @@
         <v>36</v>
       </c>
       <c r="D280" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -7298,7 +7292,7 @@
         <v>36</v>
       </c>
       <c r="D281" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -7312,7 +7306,7 @@
         <v>37</v>
       </c>
       <c r="D282" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -7326,7 +7320,7 @@
         <v>37</v>
       </c>
       <c r="D283" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -7340,7 +7334,7 @@
         <v>37</v>
       </c>
       <c r="D284" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -7354,7 +7348,7 @@
         <v>37</v>
       </c>
       <c r="D285" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -7368,7 +7362,7 @@
         <v>37</v>
       </c>
       <c r="D286" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -7382,7 +7376,7 @@
         <v>37</v>
       </c>
       <c r="D287" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -7396,7 +7390,7 @@
         <v>37</v>
       </c>
       <c r="D288" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -7410,7 +7404,7 @@
         <v>37</v>
       </c>
       <c r="D289" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -7424,7 +7418,7 @@
         <v>37</v>
       </c>
       <c r="D290" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -7438,7 +7432,7 @@
         <v>37</v>
       </c>
       <c r="D291" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -7452,7 +7446,7 @@
         <v>37</v>
       </c>
       <c r="D292" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -7466,7 +7460,7 @@
         <v>37</v>
       </c>
       <c r="D293" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
@@ -7480,7 +7474,7 @@
         <v>37</v>
       </c>
       <c r="D294" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -7494,7 +7488,7 @@
         <v>37</v>
       </c>
       <c r="D295" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
@@ -7508,7 +7502,7 @@
         <v>37</v>
       </c>
       <c r="D296" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -7522,7 +7516,7 @@
         <v>37</v>
       </c>
       <c r="D297" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -7536,7 +7530,7 @@
         <v>37</v>
       </c>
       <c r="D298" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -7550,7 +7544,7 @@
         <v>37</v>
       </c>
       <c r="D299" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -7564,7 +7558,7 @@
         <v>37</v>
       </c>
       <c r="D300" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -7578,7 +7572,7 @@
         <v>37</v>
       </c>
       <c r="D301" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
@@ -7592,7 +7586,7 @@
         <v>38</v>
       </c>
       <c r="D302" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -7606,7 +7600,7 @@
         <v>38</v>
       </c>
       <c r="D303" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
@@ -7620,7 +7614,7 @@
         <v>38</v>
       </c>
       <c r="D304" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -7634,7 +7628,7 @@
         <v>38</v>
       </c>
       <c r="D305" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -7648,7 +7642,7 @@
         <v>38</v>
       </c>
       <c r="D306" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -7662,7 +7656,7 @@
         <v>38</v>
       </c>
       <c r="D307" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -7676,7 +7670,7 @@
         <v>38</v>
       </c>
       <c r="D308" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -7690,7 +7684,7 @@
         <v>38</v>
       </c>
       <c r="D309" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -7704,7 +7698,7 @@
         <v>38</v>
       </c>
       <c r="D310" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -7718,7 +7712,7 @@
         <v>39</v>
       </c>
       <c r="D311" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -7732,7 +7726,7 @@
         <v>39</v>
       </c>
       <c r="D312" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -7746,7 +7740,7 @@
         <v>39</v>
       </c>
       <c r="D313" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
@@ -7760,7 +7754,7 @@
         <v>39</v>
       </c>
       <c r="D314" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -7774,7 +7768,7 @@
         <v>39</v>
       </c>
       <c r="D315" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
@@ -7788,7 +7782,7 @@
         <v>40</v>
       </c>
       <c r="D316" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -7802,7 +7796,7 @@
         <v>40</v>
       </c>
       <c r="D317" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -7816,7 +7810,7 @@
         <v>40</v>
       </c>
       <c r="D318" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -7830,7 +7824,7 @@
         <v>40</v>
       </c>
       <c r="D319" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -7844,7 +7838,7 @@
         <v>40</v>
       </c>
       <c r="D320" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -7858,7 +7852,7 @@
         <v>40</v>
       </c>
       <c r="D321" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -7872,7 +7866,7 @@
         <v>40</v>
       </c>
       <c r="D322" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -7886,7 +7880,7 @@
         <v>40</v>
       </c>
       <c r="D323" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -7900,7 +7894,7 @@
         <v>40</v>
       </c>
       <c r="D324" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -7914,7 +7908,7 @@
         <v>40</v>
       </c>
       <c r="D325" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -7928,7 +7922,7 @@
         <v>40</v>
       </c>
       <c r="D326" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -7942,7 +7936,7 @@
         <v>40</v>
       </c>
       <c r="D327" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -7956,7 +7950,7 @@
         <v>40</v>
       </c>
       <c r="D328" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -7970,7 +7964,7 @@
         <v>40</v>
       </c>
       <c r="D329" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -7984,7 +7978,7 @@
         <v>40</v>
       </c>
       <c r="D330" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -7998,7 +7992,7 @@
         <v>40</v>
       </c>
       <c r="D331" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -8012,7 +8006,7 @@
         <v>40</v>
       </c>
       <c r="D332" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -8026,7 +8020,7 @@
         <v>40</v>
       </c>
       <c r="D333" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -8040,7 +8034,7 @@
         <v>40</v>
       </c>
       <c r="D334" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -8054,7 +8048,7 @@
         <v>40</v>
       </c>
       <c r="D335" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -8068,7 +8062,7 @@
         <v>41</v>
       </c>
       <c r="D336" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -8082,7 +8076,7 @@
         <v>41</v>
       </c>
       <c r="D337" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -8096,7 +8090,7 @@
         <v>41</v>
       </c>
       <c r="D338" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -8110,7 +8104,7 @@
         <v>41</v>
       </c>
       <c r="D339" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -8124,7 +8118,7 @@
         <v>41</v>
       </c>
       <c r="D340" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -8138,7 +8132,7 @@
         <v>41</v>
       </c>
       <c r="D341" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -8152,7 +8146,7 @@
         <v>41</v>
       </c>
       <c r="D342" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -8166,7 +8160,7 @@
         <v>41</v>
       </c>
       <c r="D343" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -8180,7 +8174,7 @@
         <v>41</v>
       </c>
       <c r="D344" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -8194,7 +8188,7 @@
         <v>41</v>
       </c>
       <c r="D345" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -8208,7 +8202,7 @@
         <v>42</v>
       </c>
       <c r="D346" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -8222,7 +8216,7 @@
         <v>42</v>
       </c>
       <c r="D347" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -8236,7 +8230,7 @@
         <v>42</v>
       </c>
       <c r="D348" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -8250,7 +8244,7 @@
         <v>42</v>
       </c>
       <c r="D349" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -8264,7 +8258,7 @@
         <v>42</v>
       </c>
       <c r="D350" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -8278,7 +8272,7 @@
         <v>42</v>
       </c>
       <c r="D351" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -8292,7 +8286,7 @@
         <v>42</v>
       </c>
       <c r="D352" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -8306,7 +8300,7 @@
         <v>42</v>
       </c>
       <c r="D353" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -8320,7 +8314,7 @@
         <v>42</v>
       </c>
       <c r="D354" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -8334,7 +8328,7 @@
         <v>42</v>
       </c>
       <c r="D355" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -8348,7 +8342,7 @@
         <v>42</v>
       </c>
       <c r="D356" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -8362,7 +8356,7 @@
         <v>42</v>
       </c>
       <c r="D357" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -8376,7 +8370,7 @@
         <v>42</v>
       </c>
       <c r="D358" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -8390,7 +8384,7 @@
         <v>42</v>
       </c>
       <c r="D359" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -8404,7 +8398,7 @@
         <v>42</v>
       </c>
       <c r="D360" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -8418,7 +8412,7 @@
         <v>42</v>
       </c>
       <c r="D361" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -8432,7 +8426,7 @@
         <v>42</v>
       </c>
       <c r="D362" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -8446,7 +8440,7 @@
         <v>42</v>
       </c>
       <c r="D363" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -8460,7 +8454,7 @@
         <v>42</v>
       </c>
       <c r="D364" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -8474,7 +8468,7 @@
         <v>42</v>
       </c>
       <c r="D365" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -8488,7 +8482,7 @@
         <v>42</v>
       </c>
       <c r="D366" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -8502,7 +8496,7 @@
         <v>42</v>
       </c>
       <c r="D367" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -8516,7 +8510,7 @@
         <v>42</v>
       </c>
       <c r="D368" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -8530,7 +8524,7 @@
         <v>42</v>
       </c>
       <c r="D369" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -8544,7 +8538,7 @@
         <v>42</v>
       </c>
       <c r="D370" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -8558,7 +8552,7 @@
         <v>42</v>
       </c>
       <c r="D371" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -8572,7 +8566,7 @@
         <v>42</v>
       </c>
       <c r="D372" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -8586,7 +8580,7 @@
         <v>42</v>
       </c>
       <c r="D373" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -8600,7 +8594,7 @@
         <v>42</v>
       </c>
       <c r="D374" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -8614,7 +8608,7 @@
         <v>42</v>
       </c>
       <c r="D375" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -8628,7 +8622,7 @@
         <v>42</v>
       </c>
       <c r="D376" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -8642,7 +8636,7 @@
         <v>42</v>
       </c>
       <c r="D377" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -8656,7 +8650,7 @@
         <v>42</v>
       </c>
       <c r="D378" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -8670,7 +8664,7 @@
         <v>42</v>
       </c>
       <c r="D379" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -8684,7 +8678,7 @@
         <v>42</v>
       </c>
       <c r="D380" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -8698,7 +8692,7 @@
         <v>42</v>
       </c>
       <c r="D381" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -8712,7 +8706,7 @@
         <v>42</v>
       </c>
       <c r="D382" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -8726,7 +8720,7 @@
         <v>42</v>
       </c>
       <c r="D383" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -8740,7 +8734,7 @@
         <v>42</v>
       </c>
       <c r="D384" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
@@ -8754,7 +8748,7 @@
         <v>42</v>
       </c>
       <c r="D385" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
@@ -8768,7 +8762,7 @@
         <v>42</v>
       </c>
       <c r="D386" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
@@ -8782,7 +8776,7 @@
         <v>42</v>
       </c>
       <c r="D387" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -8796,7 +8790,7 @@
         <v>42</v>
       </c>
       <c r="D388" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -8810,7 +8804,7 @@
         <v>42</v>
       </c>
       <c r="D389" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -8824,7 +8818,7 @@
         <v>42</v>
       </c>
       <c r="D390" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -8838,7 +8832,7 @@
         <v>42</v>
       </c>
       <c r="D391" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
@@ -8852,7 +8846,7 @@
         <v>42</v>
       </c>
       <c r="D392" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
@@ -8866,7 +8860,7 @@
         <v>42</v>
       </c>
       <c r="D393" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
@@ -8880,7 +8874,7 @@
         <v>42</v>
       </c>
       <c r="D394" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -8894,7 +8888,7 @@
         <v>42</v>
       </c>
       <c r="D395" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -8908,7 +8902,7 @@
         <v>43</v>
       </c>
       <c r="D396" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -8922,7 +8916,7 @@
         <v>43</v>
       </c>
       <c r="D397" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
@@ -8936,7 +8930,7 @@
         <v>43</v>
       </c>
       <c r="D398" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -8950,7 +8944,7 @@
         <v>43</v>
       </c>
       <c r="D399" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -8964,7 +8958,7 @@
         <v>43</v>
       </c>
       <c r="D400" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
@@ -8978,7 +8972,7 @@
         <v>43</v>
       </c>
       <c r="D401" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -8992,7 +8986,7 @@
         <v>43</v>
       </c>
       <c r="D402" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
@@ -9006,7 +9000,7 @@
         <v>43</v>
       </c>
       <c r="D403" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -9020,7 +9014,7 @@
         <v>43</v>
       </c>
       <c r="D404" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
@@ -9034,7 +9028,7 @@
         <v>45</v>
       </c>
       <c r="D405" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -9048,7 +9042,7 @@
         <v>45</v>
       </c>
       <c r="D406" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -9062,7 +9056,7 @@
         <v>46</v>
       </c>
       <c r="D407" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
@@ -9076,7 +9070,7 @@
         <v>46</v>
       </c>
       <c r="D408" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
@@ -9090,7 +9084,7 @@
         <v>47</v>
       </c>
       <c r="D409" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
@@ -9104,7 +9098,7 @@
         <v>47</v>
       </c>
       <c r="D410" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
@@ -9118,7 +9112,7 @@
         <v>48</v>
       </c>
       <c r="D411" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
@@ -9132,7 +9126,7 @@
         <v>49</v>
       </c>
       <c r="D412" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
@@ -9146,7 +9140,7 @@
         <v>50</v>
       </c>
       <c r="D413" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
@@ -9160,7 +9154,7 @@
         <v>51</v>
       </c>
       <c r="D414" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
@@ -9174,7 +9168,7 @@
         <v>54</v>
       </c>
       <c r="D415" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
@@ -9188,7 +9182,7 @@
         <v>54</v>
       </c>
       <c r="D416" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
@@ -9202,7 +9196,7 @@
         <v>55</v>
       </c>
       <c r="D417" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -9216,7 +9210,7 @@
         <v>55</v>
       </c>
       <c r="D418" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
@@ -9230,7 +9224,7 @@
         <v>56</v>
       </c>
       <c r="D419" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
@@ -9244,7 +9238,7 @@
         <v>56</v>
       </c>
       <c r="D420" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
@@ -9258,7 +9252,7 @@
         <v>56</v>
       </c>
       <c r="D421" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
@@ -9272,7 +9266,7 @@
         <v>57</v>
       </c>
       <c r="D422" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
@@ -9286,7 +9280,7 @@
         <v>57</v>
       </c>
       <c r="D423" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -9300,7 +9294,7 @@
         <v>57</v>
       </c>
       <c r="D424" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
@@ -9314,7 +9308,7 @@
         <v>57</v>
       </c>
       <c r="D425" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
@@ -9328,7 +9322,7 @@
         <v>58</v>
       </c>
       <c r="D426" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
@@ -9342,7 +9336,7 @@
         <v>58</v>
       </c>
       <c r="D427" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
@@ -9356,7 +9350,7 @@
         <v>58</v>
       </c>
       <c r="D428" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
@@ -9370,7 +9364,7 @@
         <v>58</v>
       </c>
       <c r="D429" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
@@ -9384,7 +9378,7 @@
         <v>59</v>
       </c>
       <c r="D430" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
@@ -9398,7 +9392,7 @@
         <v>59</v>
       </c>
       <c r="D431" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
@@ -9412,7 +9406,7 @@
         <v>59</v>
       </c>
       <c r="D432" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
@@ -9426,7 +9420,7 @@
         <v>59</v>
       </c>
       <c r="D433" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -9440,7 +9434,7 @@
         <v>60</v>
       </c>
       <c r="D434" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
@@ -9454,7 +9448,7 @@
         <v>60</v>
       </c>
       <c r="D435" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -9468,7 +9462,7 @@
         <v>60</v>
       </c>
       <c r="D436" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
@@ -9482,7 +9476,7 @@
         <v>60</v>
       </c>
       <c r="D437" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
@@ -9496,7 +9490,7 @@
         <v>61</v>
       </c>
       <c r="D438" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
@@ -9510,7 +9504,7 @@
         <v>61</v>
       </c>
       <c r="D439" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
@@ -9524,7 +9518,7 @@
         <v>61</v>
       </c>
       <c r="D440" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
@@ -9538,7 +9532,7 @@
         <v>61</v>
       </c>
       <c r="D441" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -9552,7 +9546,7 @@
         <v>61</v>
       </c>
       <c r="D442" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
@@ -9566,7 +9560,7 @@
         <v>61</v>
       </c>
       <c r="D443" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -9580,7 +9574,7 @@
         <v>62</v>
       </c>
       <c r="D444" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -9594,7 +9588,7 @@
         <v>62</v>
       </c>
       <c r="D445" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -9608,7 +9602,7 @@
         <v>62</v>
       </c>
       <c r="D446" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -9622,7 +9616,7 @@
         <v>63</v>
       </c>
       <c r="D447" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -9636,7 +9630,7 @@
         <v>63</v>
       </c>
       <c r="D448" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -9650,7 +9644,7 @@
         <v>63</v>
       </c>
       <c r="D449" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
@@ -9664,7 +9658,7 @@
         <v>64</v>
       </c>
       <c r="D450" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
@@ -9678,7 +9672,7 @@
         <v>64</v>
       </c>
       <c r="D451" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
@@ -9692,7 +9686,7 @@
         <v>64</v>
       </c>
       <c r="D452" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
@@ -9706,7 +9700,7 @@
         <v>65</v>
       </c>
       <c r="D453" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
@@ -9720,7 +9714,7 @@
         <v>65</v>
       </c>
       <c r="D454" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
@@ -9734,7 +9728,7 @@
         <v>65</v>
       </c>
       <c r="D455" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
@@ -9748,7 +9742,7 @@
         <v>66</v>
       </c>
       <c r="D456" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -9762,7 +9756,7 @@
         <v>66</v>
       </c>
       <c r="D457" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
@@ -9776,7 +9770,7 @@
         <v>67</v>
       </c>
       <c r="D458" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -9790,7 +9784,7 @@
         <v>67</v>
       </c>
       <c r="D459" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
@@ -9804,7 +9798,7 @@
         <v>68</v>
       </c>
       <c r="D460" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -9818,7 +9812,7 @@
         <v>69</v>
       </c>
       <c r="D461" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -9832,7 +9826,7 @@
         <v>69</v>
       </c>
       <c r="D462" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -9846,7 +9840,7 @@
         <v>69</v>
       </c>
       <c r="D463" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.25">
@@ -9860,7 +9854,7 @@
         <v>70</v>
       </c>
       <c r="D464" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
@@ -9874,7 +9868,7 @@
         <v>70</v>
       </c>
       <c r="D465" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
@@ -9888,7 +9882,7 @@
         <v>71</v>
       </c>
       <c r="D466" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
@@ -9902,7 +9896,7 @@
         <v>71</v>
       </c>
       <c r="D467" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
@@ -9916,7 +9910,7 @@
         <v>71</v>
       </c>
       <c r="D468" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -9930,7 +9924,7 @@
         <v>71</v>
       </c>
       <c r="D469" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -9944,7 +9938,7 @@
         <v>72</v>
       </c>
       <c r="D470" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -9958,7 +9952,7 @@
         <v>73</v>
       </c>
       <c r="D471" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
@@ -9972,7 +9966,7 @@
         <v>74</v>
       </c>
       <c r="D472" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
@@ -9986,7 +9980,7 @@
         <v>74</v>
       </c>
       <c r="D473" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
@@ -10000,7 +9994,7 @@
         <v>75</v>
       </c>
       <c r="D474" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
@@ -10014,7 +10008,7 @@
         <v>76</v>
       </c>
       <c r="D475" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
@@ -10028,7 +10022,7 @@
         <v>77</v>
       </c>
       <c r="D476" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -10042,7 +10036,7 @@
         <v>77</v>
       </c>
       <c r="D477" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
@@ -10056,7 +10050,7 @@
         <v>77</v>
       </c>
       <c r="D478" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
@@ -10070,7 +10064,7 @@
         <v>77</v>
       </c>
       <c r="D479" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -10084,7 +10078,7 @@
         <v>79</v>
       </c>
       <c r="D480" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -10098,7 +10092,7 @@
         <v>79</v>
       </c>
       <c r="D481" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
@@ -10112,7 +10106,7 @@
         <v>79</v>
       </c>
       <c r="D482" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
@@ -10126,7 +10120,7 @@
         <v>79</v>
       </c>
       <c r="D483" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
@@ -10140,7 +10134,7 @@
         <v>79</v>
       </c>
       <c r="D484" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
@@ -10154,7 +10148,7 @@
         <v>79</v>
       </c>
       <c r="D485" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
@@ -10168,7 +10162,7 @@
         <v>80</v>
       </c>
       <c r="D486" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
@@ -10182,7 +10176,7 @@
         <v>80</v>
       </c>
       <c r="D487" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -10196,7 +10190,7 @@
         <v>80</v>
       </c>
       <c r="D488" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -10210,7 +10204,7 @@
         <v>81</v>
       </c>
       <c r="D489" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -10224,7 +10218,7 @@
         <v>81</v>
       </c>
       <c r="D490" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -10238,7 +10232,7 @@
         <v>81</v>
       </c>
       <c r="D491" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -10252,7 +10246,7 @@
         <v>82</v>
       </c>
       <c r="D492" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -10266,7 +10260,7 @@
         <v>83</v>
       </c>
       <c r="D493" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
@@ -10280,7 +10274,7 @@
         <v>85</v>
       </c>
       <c r="D494" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
@@ -10294,7 +10288,7 @@
         <v>85</v>
       </c>
       <c r="D495" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.25">
@@ -10308,7 +10302,7 @@
         <v>85</v>
       </c>
       <c r="D496" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
@@ -10322,7 +10316,7 @@
         <v>85</v>
       </c>
       <c r="D497" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
@@ -10336,7 +10330,7 @@
         <v>85</v>
       </c>
       <c r="D498" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
@@ -10350,7 +10344,7 @@
         <v>85</v>
       </c>
       <c r="D499" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
@@ -10364,7 +10358,7 @@
         <v>86</v>
       </c>
       <c r="D500" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
@@ -10378,7 +10372,7 @@
         <v>86</v>
       </c>
       <c r="D501" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.25">
@@ -10392,7 +10386,7 @@
         <v>87</v>
       </c>
       <c r="D502" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
@@ -10406,7 +10400,7 @@
         <v>87</v>
       </c>
       <c r="D503" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
@@ -10420,7 +10414,7 @@
         <v>89</v>
       </c>
       <c r="D504" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.25">
@@ -10434,7 +10428,7 @@
         <v>89</v>
       </c>
       <c r="D505" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
@@ -10448,7 +10442,7 @@
         <v>89</v>
       </c>
       <c r="D506" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
@@ -10462,7 +10456,7 @@
         <v>89</v>
       </c>
       <c r="D507" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
@@ -10476,7 +10470,7 @@
         <v>89</v>
       </c>
       <c r="D508" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
@@ -10490,7 +10484,7 @@
         <v>89</v>
       </c>
       <c r="D509" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.25">
@@ -10504,7 +10498,7 @@
         <v>90</v>
       </c>
       <c r="D510" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
@@ -10518,7 +10512,7 @@
         <v>90</v>
       </c>
       <c r="D511" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -10532,7 +10526,7 @@
         <v>91</v>
       </c>
       <c r="D512" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
@@ -10546,7 +10540,7 @@
         <v>91</v>
       </c>
       <c r="D513" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
@@ -10560,7 +10554,7 @@
         <v>93</v>
       </c>
       <c r="D514" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
@@ -10574,7 +10568,7 @@
         <v>93</v>
       </c>
       <c r="D515" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
@@ -10588,7 +10582,7 @@
         <v>94</v>
       </c>
       <c r="D516" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
@@ -10602,7 +10596,7 @@
         <v>94</v>
       </c>
       <c r="D517" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
@@ -10616,7 +10610,7 @@
         <v>95</v>
       </c>
       <c r="D518" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
@@ -10630,7 +10624,7 @@
         <v>95</v>
       </c>
       <c r="D519" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
@@ -10644,7 +10638,7 @@
         <v>96</v>
       </c>
       <c r="D520" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
@@ -10658,7 +10652,7 @@
         <v>96</v>
       </c>
       <c r="D521" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
@@ -10672,7 +10666,7 @@
         <v>97</v>
       </c>
       <c r="D522" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
@@ -10686,7 +10680,7 @@
         <v>100</v>
       </c>
       <c r="D523" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
@@ -10798,7 +10792,7 @@
         <v>103</v>
       </c>
       <c r="D531" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
@@ -10812,7 +10806,7 @@
         <v>104</v>
       </c>
       <c r="D532" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
@@ -10826,7 +10820,7 @@
         <v>104</v>
       </c>
       <c r="D533" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
@@ -10840,7 +10834,7 @@
         <v>104</v>
       </c>
       <c r="D534" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
@@ -10854,7 +10848,7 @@
         <v>104</v>
       </c>
       <c r="D535" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
@@ -10868,7 +10862,7 @@
         <v>104</v>
       </c>
       <c r="D536" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
@@ -10882,7 +10876,7 @@
         <v>105</v>
       </c>
       <c r="D537" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
@@ -10896,7 +10890,7 @@
         <v>106</v>
       </c>
       <c r="D538" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
@@ -10910,7 +10904,7 @@
         <v>106</v>
       </c>
       <c r="D539" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
@@ -10924,7 +10918,7 @@
         <v>107</v>
       </c>
       <c r="D540" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
@@ -10938,7 +10932,7 @@
         <v>108</v>
       </c>
       <c r="D541" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
@@ -10952,7 +10946,7 @@
         <v>108</v>
       </c>
       <c r="D542" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
@@ -10966,7 +10960,7 @@
         <v>109</v>
       </c>
       <c r="D543" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
@@ -10980,7 +10974,7 @@
         <v>109</v>
       </c>
       <c r="D544" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
@@ -10994,7 +10988,7 @@
         <v>110</v>
       </c>
       <c r="D545" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
@@ -11008,7 +11002,7 @@
         <v>110</v>
       </c>
       <c r="D546" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
@@ -11022,7 +11016,7 @@
         <v>111</v>
       </c>
       <c r="D547" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
@@ -11036,7 +11030,7 @@
         <v>111</v>
       </c>
       <c r="D548" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
@@ -11050,7 +11044,7 @@
         <v>112</v>
       </c>
       <c r="D549" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
@@ -11064,7 +11058,7 @@
         <v>112</v>
       </c>
       <c r="D550" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
@@ -11078,7 +11072,7 @@
         <v>113</v>
       </c>
       <c r="D551" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
@@ -11092,7 +11086,7 @@
         <v>113</v>
       </c>
       <c r="D552" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
@@ -11106,7 +11100,7 @@
         <v>113</v>
       </c>
       <c r="D553" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.25">
@@ -11120,7 +11114,7 @@
         <v>113</v>
       </c>
       <c r="D554" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.25">
@@ -11134,7 +11128,7 @@
         <v>114</v>
       </c>
       <c r="D555" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
@@ -11148,7 +11142,7 @@
         <v>114</v>
       </c>
       <c r="D556" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.25">
@@ -11162,7 +11156,7 @@
         <v>114</v>
       </c>
       <c r="D557" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
@@ -11176,7 +11170,7 @@
         <v>114</v>
       </c>
       <c r="D558" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
@@ -11190,7 +11184,7 @@
         <v>114</v>
       </c>
       <c r="D559" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
@@ -11204,7 +11198,7 @@
         <v>114</v>
       </c>
       <c r="D560" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
@@ -11218,7 +11212,7 @@
         <v>114</v>
       </c>
       <c r="D561" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
@@ -11232,7 +11226,7 @@
         <v>114</v>
       </c>
       <c r="D562" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
@@ -11246,7 +11240,7 @@
         <v>115</v>
       </c>
       <c r="D563" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
@@ -11260,7 +11254,7 @@
         <v>115</v>
       </c>
       <c r="D564" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.25">
@@ -11274,7 +11268,7 @@
         <v>116</v>
       </c>
       <c r="D565" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
@@ -11288,7 +11282,7 @@
         <v>116</v>
       </c>
       <c r="D566" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.25">
@@ -11302,7 +11296,7 @@
         <v>116</v>
       </c>
       <c r="D567" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.25">
@@ -11316,7 +11310,7 @@
         <v>116</v>
       </c>
       <c r="D568" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
@@ -11330,7 +11324,7 @@
         <v>117</v>
       </c>
       <c r="D569" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
@@ -11344,7 +11338,7 @@
         <v>118</v>
       </c>
       <c r="D570" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.25">
@@ -11358,7 +11352,7 @@
         <v>119</v>
       </c>
       <c r="D571" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.25">
@@ -11372,7 +11366,7 @@
         <v>121</v>
       </c>
       <c r="D572" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.25">
@@ -11386,7 +11380,7 @@
         <v>122</v>
       </c>
       <c r="D573" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.25">
@@ -11400,7 +11394,7 @@
         <v>123</v>
       </c>
       <c r="D574" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.25">
@@ -11414,7 +11408,7 @@
         <v>123</v>
       </c>
       <c r="D575" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.25">
@@ -11428,7 +11422,7 @@
         <v>124</v>
       </c>
       <c r="D576" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.25">
@@ -11442,7 +11436,7 @@
         <v>124</v>
       </c>
       <c r="D577" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.25">
@@ -11456,7 +11450,7 @@
         <v>125</v>
       </c>
       <c r="D578" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -19855,15 +19849,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4EC50-856C-4ED2-9A0A-F74D8668D6FA}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -19877,7 +19872,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -20038,7 +20033,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>806</v>
@@ -20050,7 +20045,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>807</v>
@@ -20062,7 +20057,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>808</v>
@@ -20074,57 +20069,57 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>810</v>
+      </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="C19" s="1" t="s">
         <v>811</v>
       </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>812</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>813</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>814</v>
@@ -20136,7 +20131,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>815</v>
@@ -20148,69 +20143,69 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>816</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>817</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>819</v>
+      </c>
       <c r="D26" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="C27" s="1" t="s">
         <v>820</v>
       </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>821</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>822</v>
@@ -20222,7 +20217,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>823</v>
@@ -20234,7 +20229,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>824</v>
@@ -20246,7 +20241,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>825</v>
@@ -20258,7 +20253,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>826</v>
@@ -20270,7 +20265,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>827</v>
@@ -20282,33 +20277,33 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>944</v>
+      </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>946</v>
-      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>830</v>
@@ -20320,19 +20315,19 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>831</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>832</v>
@@ -20344,7 +20339,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>833</v>
@@ -20356,7 +20351,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>834</v>
@@ -20368,7 +20363,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>835</v>
@@ -20380,33 +20375,33 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>837</v>
+      </c>
       <c r="D43" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="C44" s="1" t="s">
         <v>838</v>
       </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>839</v>
@@ -20418,7 +20413,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>840</v>
@@ -20430,7 +20425,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>841</v>
@@ -20442,95 +20437,95 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>842</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>843</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>844</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>845</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="C52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>847</v>
+      </c>
       <c r="D52" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D53" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="C54" s="1" t="s">
         <v>850</v>
       </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>851</v>
@@ -20542,31 +20537,31 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>852</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>853</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>854</v>
@@ -20578,19 +20573,19 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>855</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>856</v>
@@ -20602,7 +20597,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>857</v>
@@ -20614,7 +20609,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>858</v>
@@ -20626,31 +20621,31 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>859</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>860</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>861</v>
@@ -20662,31 +20657,31 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>862</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>863</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>864</v>
@@ -20698,45 +20693,45 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>865</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="C70" s="1"/>
+      <c r="C70" s="1" t="s">
+        <v>867</v>
+      </c>
       <c r="D70" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>867</v>
-      </c>
-      <c r="C71" s="1" t="s">
         <v>868</v>
       </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>869</v>
@@ -20748,31 +20743,31 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>870</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>871</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>872</v>
@@ -20784,7 +20779,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>873</v>
@@ -20796,7 +20791,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>874</v>
@@ -20808,70 +20803,70 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>875</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>876</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>877</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>878</v>
+        <v>759</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>759</v>
+        <v>879</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1">
@@ -20880,19 +20875,19 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>880</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>881</v>
@@ -20904,7 +20899,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>882</v>
@@ -20916,7 +20911,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>883</v>
@@ -20928,7 +20923,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>884</v>
@@ -20940,7 +20935,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>885</v>
@@ -20952,7 +20947,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>886</v>
@@ -20964,7 +20959,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>887</v>
@@ -20976,119 +20971,119 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>888</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>889</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>890</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>891</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="C96" s="1"/>
+      <c r="C96" s="1" t="s">
+        <v>945</v>
+      </c>
       <c r="D96" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="C97" s="1"/>
+      <c r="C97" s="1" t="s">
+        <v>946</v>
+      </c>
       <c r="D97" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>947</v>
-      </c>
+      <c r="C98" s="1"/>
       <c r="D98" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>948</v>
-      </c>
+      <c r="C99" s="1"/>
       <c r="D99" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>896</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>897</v>
@@ -21100,61 +21095,37 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>898</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>899</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>900</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>124</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>901</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>125</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>902</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1">
         <v>1</v>
       </c>
     </row>
@@ -21178,10 +21149,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
@@ -21192,13 +21163,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -21206,13 +21177,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -21220,13 +21191,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -21234,13 +21205,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -21248,13 +21219,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -21262,7 +21233,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -21274,7 +21245,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -21286,7 +21257,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -21317,7 +21288,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
@@ -21328,10 +21299,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -21339,10 +21310,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -21350,7 +21321,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
   </sheetData>
@@ -21377,13 +21348,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -21391,10 +21362,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D2" t="s">
         <v>98</v>
@@ -21405,10 +21376,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C3" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D3" t="s">
         <v>98</v>
@@ -21419,10 +21390,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C4" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="D4" t="s">
         <v>98</v>
@@ -21433,10 +21404,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C5" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D5" t="s">
         <v>98</v>
@@ -21447,10 +21418,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C6" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D6" t="s">
         <v>98</v>
@@ -21461,10 +21432,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C7" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D7" t="s">
         <v>98</v>
@@ -21475,7 +21446,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C8" t="s">
         <v>98</v>
@@ -21489,7 +21460,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C9" t="s">
         <v>98</v>
@@ -21503,7 +21474,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C10" t="s">
         <v>98</v>
@@ -21517,7 +21488,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C11" t="s">
         <v>98</v>
@@ -21546,7 +21517,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -21557,10 +21528,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -21568,10 +21539,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C3" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -21579,10 +21550,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C4" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -21590,10 +21561,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C5" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -21601,10 +21572,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C6" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -21612,10 +21583,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -21623,10 +21594,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C8" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -21634,10 +21605,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C9" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -21645,10 +21616,10 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C10" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -21656,10 +21627,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C11" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -21667,7 +21638,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C12" t="s">
         <v>98</v>
@@ -21678,7 +21649,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C13" t="s">
         <v>98</v>
@@ -21689,7 +21660,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C14" t="s">
         <v>98</v>
@@ -21700,7 +21671,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C15" t="s">
         <v>98</v>

</xml_diff>